<commit_message>
Update test case overzicht surf.xlsx
</commit_message>
<xml_diff>
--- a/test case overzicht surf.xlsx
+++ b/test case overzicht surf.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="BadgeClass CRUD" sheetId="1" state="visible" r:id="rId3"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="96">
   <si>
     <t xml:space="preserve">Onderwijsinstelling</t>
   </si>
@@ -147,6 +147,9 @@
     <t xml:space="preserve">Actie system admin</t>
   </si>
   <si>
+    <t xml:space="preserve">Student → EditBadge</t>
+  </si>
+  <si>
     <t xml:space="preserve">Badge delen</t>
   </si>
   <si>
@@ -162,6 +165,9 @@
     <t xml:space="preserve">Badge intrekken - HBO</t>
   </si>
   <si>
+    <t xml:space="preserve">Student → BadgeRemoval</t>
+  </si>
+  <si>
     <t xml:space="preserve">Badge intrekken - Uni</t>
   </si>
   <si>
@@ -198,6 +204,9 @@
     <t xml:space="preserve">Verwijderen</t>
   </si>
   <si>
+    <t xml:space="preserve">Teacher → BadgeInteraction → BadgeCreation</t>
+  </si>
+  <si>
     <t xml:space="preserve">Backpackpage → Login</t>
   </si>
   <si>
@@ -292,6 +301,9 @@
   </si>
   <si>
     <t xml:space="preserve">Harvard-example.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read by Teacher → BadgeInteraction → SeeBadge</t>
   </si>
   <si>
     <t xml:space="preserve">Read by Student → BasicsCatalog</t>
@@ -311,13 +323,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -336,17 +347,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="13">
@@ -792,6 +795,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -808,11 +815,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -951,14 +954,14 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -966,67 +969,25 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -1045,35 +1006,11 @@
           <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-          </a:schemeClr>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
@@ -1085,7 +1022,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:R35"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H44" activeCellId="0" sqref="H44"/>
@@ -1105,7 +1042,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="10.57"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <f aca="false">COUNT(A5:A34)</f>
         <v>30</v>
@@ -1134,7 +1073,7 @@
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
@@ -1181,7 +1120,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="n">
         <v>1</v>
       </c>
@@ -1210,7 +1149,7 @@
       <c r="Q5" s="14"/>
       <c r="R5" s="15"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <v>2</v>
       </c>
@@ -1232,7 +1171,7 @@
       </c>
       <c r="R6" s="19"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <v>3</v>
       </c>
@@ -1254,7 +1193,7 @@
       </c>
       <c r="R7" s="19"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
         <v>4</v>
       </c>
@@ -1275,7 +1214,7 @@
       </c>
       <c r="R8" s="19"/>
     </row>
-    <row r="9" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="n">
         <v>5</v>
       </c>
@@ -1304,7 +1243,7 @@
       <c r="Q9" s="14"/>
       <c r="R9" s="15"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
         <v>6</v>
       </c>
@@ -1327,7 +1266,7 @@
       </c>
       <c r="R10" s="19"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
         <v>7</v>
       </c>
@@ -1350,7 +1289,7 @@
       </c>
       <c r="R11" s="19"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
         <v>8</v>
       </c>
@@ -1372,7 +1311,7 @@
       </c>
       <c r="R12" s="19"/>
     </row>
-    <row r="13" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="12" t="n">
         <v>9</v>
       </c>
@@ -1401,7 +1340,7 @@
       <c r="Q13" s="14"/>
       <c r="R13" s="15"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
         <v>10</v>
       </c>
@@ -1423,7 +1362,7 @@
       </c>
       <c r="R14" s="19"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
         <v>11</v>
       </c>
@@ -1445,7 +1384,7 @@
       </c>
       <c r="R15" s="19"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
         <v>12</v>
       </c>
@@ -1466,7 +1405,7 @@
       </c>
       <c r="R16" s="19"/>
     </row>
-    <row r="17" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="12" t="n">
         <v>13</v>
       </c>
@@ -1495,7 +1434,7 @@
       <c r="Q17" s="14"/>
       <c r="R17" s="15"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
         <v>14</v>
       </c>
@@ -1518,7 +1457,7 @@
       </c>
       <c r="R18" s="19"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
         <v>15</v>
       </c>
@@ -1541,7 +1480,7 @@
       </c>
       <c r="R19" s="19"/>
     </row>
-    <row r="20" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="12" t="n">
         <v>16</v>
       </c>
@@ -1570,7 +1509,7 @@
       <c r="Q20" s="14"/>
       <c r="R20" s="15"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
         <v>17</v>
       </c>
@@ -1594,7 +1533,7 @@
       </c>
       <c r="R21" s="19"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
         <v>18</v>
       </c>
@@ -1618,7 +1557,7 @@
       </c>
       <c r="R22" s="19"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="12" t="n">
         <v>19</v>
       </c>
@@ -1648,7 +1587,7 @@
       <c r="Q23" s="14"/>
       <c r="R23" s="15"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
         <v>20</v>
       </c>
@@ -1671,7 +1610,7 @@
       </c>
       <c r="R24" s="19"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
         <v>21</v>
       </c>
@@ -1694,7 +1633,7 @@
       </c>
       <c r="R25" s="19"/>
     </row>
-    <row r="26" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="12" t="n">
         <v>22</v>
       </c>
@@ -1723,7 +1662,7 @@
       <c r="Q26" s="14"/>
       <c r="R26" s="15"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
         <v>23</v>
       </c>
@@ -1746,7 +1685,7 @@
       </c>
       <c r="R27" s="19"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
         <v>24</v>
       </c>
@@ -1769,7 +1708,7 @@
       </c>
       <c r="R28" s="19"/>
     </row>
-    <row r="29" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="12" t="n">
         <v>25</v>
       </c>
@@ -1798,7 +1737,7 @@
       <c r="Q29" s="14"/>
       <c r="R29" s="15"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="n">
         <v>26</v>
       </c>
@@ -1822,7 +1761,7 @@
       </c>
       <c r="R30" s="19"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="n">
         <v>27</v>
       </c>
@@ -1847,7 +1786,7 @@
       </c>
       <c r="R31" s="19"/>
     </row>
-    <row r="32" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="12" t="n">
         <v>28</v>
       </c>
@@ -1876,7 +1815,7 @@
       <c r="Q32" s="14"/>
       <c r="R32" s="15"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="n">
         <v>29</v>
       </c>
@@ -1899,7 +1838,7 @@
       </c>
       <c r="R33" s="19"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="n">
         <v>30</v>
       </c>
@@ -1922,7 +1861,7 @@
       </c>
       <c r="R34" s="19"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="24"/>
       <c r="C35" s="25"/>
       <c r="D35" s="25"/>
@@ -1961,7 +1900,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:O18"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L11" activeCellId="0" sqref="L11"/>
@@ -1981,7 +1920,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="11.72"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="3" t="s">
         <v>20</v>
       </c>
@@ -2047,7 +1988,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="3"/>
       <c r="C5" s="28"/>
       <c r="D5" s="30"/>
@@ -2058,7 +1999,7 @@
       <c r="N5" s="28"/>
       <c r="O5" s="11"/>
     </row>
-    <row r="6" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
         <v>19</v>
       </c>
@@ -2082,7 +2023,7 @@
       <c r="N6" s="14"/>
       <c r="O6" s="21"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -2102,7 +2043,7 @@
       <c r="N7" s="1"/>
       <c r="O7" s="20"/>
     </row>
-    <row r="8" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
         <v>19</v>
       </c>
@@ -2126,7 +2067,7 @@
       <c r="N8" s="14"/>
       <c r="O8" s="21"/>
     </row>
-    <row r="9" s="31" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="31" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="31" t="s">
         <v>19</v>
       </c>
@@ -2150,7 +2091,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" s="36" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" s="36" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="36" t="s">
         <v>19</v>
       </c>
@@ -2174,7 +2115,7 @@
       <c r="N10" s="22"/>
       <c r="O10" s="20"/>
     </row>
-    <row r="11" s="36" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" s="36" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="36" t="s">
         <v>19</v>
       </c>
@@ -2198,7 +2139,7 @@
       <c r="N11" s="22"/>
       <c r="O11" s="20"/>
     </row>
-    <row r="12" s="36" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" s="36" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="36" t="s">
         <v>19</v>
       </c>
@@ -2222,7 +2163,7 @@
       <c r="N12" s="22"/>
       <c r="O12" s="20"/>
     </row>
-    <row r="13" s="31" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" s="31" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="31" t="s">
         <v>19</v>
       </c>
@@ -2246,7 +2187,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" s="36" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" s="36" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="36" t="s">
         <v>19</v>
       </c>
@@ -2270,7 +2211,7 @@
       <c r="N14" s="22"/>
       <c r="O14" s="20"/>
     </row>
-    <row r="15" s="36" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" s="36" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="36" t="s">
         <v>19</v>
       </c>
@@ -2294,7 +2235,7 @@
       <c r="N15" s="22"/>
       <c r="O15" s="20"/>
     </row>
-    <row r="16" s="36" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" s="36" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="36" t="s">
         <v>19</v>
       </c>
@@ -2318,7 +2259,7 @@
       <c r="N16" s="22"/>
       <c r="O16" s="20"/>
     </row>
-    <row r="17" s="31" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" s="31" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="31" t="s">
         <v>19</v>
       </c>
@@ -2342,7 +2283,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="24"/>
       <c r="C18" s="25"/>
       <c r="D18" s="26"/>
@@ -2378,10 +2319,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:J17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2396,6 +2337,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="23.43"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="37" t="s">
         <v>28</v>
@@ -2408,7 +2350,7 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
@@ -2431,7 +2373,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="3"/>
       <c r="E4" s="28"/>
       <c r="F4" s="28"/>
@@ -2441,7 +2383,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="39" t="s">
         <v>32</v>
       </c>
@@ -2459,7 +2401,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="41" t="s">
         <v>35</v>
       </c>
@@ -2477,7 +2419,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="39" t="s">
         <v>32</v>
       </c>
@@ -2495,9 +2437,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="41" t="s">
+        <v>40</v>
+      </c>
       <c r="B8" s="38" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="1"/>
@@ -2507,9 +2452,9 @@
       </c>
       <c r="H8" s="19"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="40" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="1" t="s">
@@ -2519,9 +2464,9 @@
       <c r="G9" s="1"/>
       <c r="H9" s="19"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="40" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="1"/>
@@ -2531,9 +2476,9 @@
       <c r="G10" s="1"/>
       <c r="H10" s="19"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="40" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="1"/>
@@ -2543,9 +2488,9 @@
       </c>
       <c r="H11" s="19"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="40" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="1"/>
@@ -2555,9 +2500,12 @@
       <c r="G12" s="1"/>
       <c r="H12" s="19"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="41" t="s">
+        <v>46</v>
+      </c>
       <c r="B13" s="40" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="1"/>
@@ -2567,12 +2515,12 @@
       <c r="G13" s="1"/>
       <c r="H13" s="19"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="39" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="40" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>19</v>
@@ -2582,9 +2530,9 @@
       <c r="G14" s="1"/>
       <c r="H14" s="19"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="42" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="1"/>
@@ -2594,12 +2542,12 @@
       <c r="G15" s="1"/>
       <c r="H15" s="19"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="44" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="43" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="1"/>
@@ -2609,7 +2557,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="24"/>
       <c r="E17" s="25"/>
       <c r="F17" s="25"/>
@@ -2635,15 +2583,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:R19"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="32.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="37.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="18.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="35"/>
@@ -2658,19 +2606,21 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="22.14"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="36" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="H3" s="46" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I3" s="46"/>
       <c r="J3" s="46"/>
@@ -2682,30 +2632,30 @@
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="L4" s="9" t="s">
         <v>15</v>
@@ -2726,7 +2676,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="47"/>
       <c r="F5" s="20"/>
       <c r="H5" s="47"/>
@@ -2740,7 +2690,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="44" t="s">
         <v>27</v>
       </c>
@@ -2767,7 +2717,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="44" t="s">
         <v>27</v>
       </c>
@@ -2794,7 +2744,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="44" t="s">
         <v>27</v>
       </c>
@@ -2818,7 +2768,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
       <c r="B9" s="54"/>
       <c r="C9" s="55" t="s">
@@ -2840,7 +2790,7 @@
       <c r="O9" s="1"/>
       <c r="P9" s="19"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
       <c r="B10" s="54"/>
       <c r="C10" s="55" t="s">
@@ -2862,7 +2812,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="19"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1"/>
       <c r="B11" s="54"/>
       <c r="C11" s="55" t="s">
@@ -2884,16 +2834,18 @@
       <c r="O11" s="1"/>
       <c r="P11" s="19"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="59" t="s">
+        <v>59</v>
+      </c>
       <c r="B12" s="54"/>
       <c r="C12" s="49"/>
-      <c r="D12" s="59" t="s">
+      <c r="D12" s="60" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="49"/>
       <c r="F12" s="50"/>
-      <c r="H12" s="60" t="s">
+      <c r="H12" s="61" t="s">
         <v>19</v>
       </c>
       <c r="I12" s="1"/>
@@ -2906,17 +2858,19 @@
       <c r="O12" s="1"/>
       <c r="P12" s="19"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="59" t="s">
+        <v>59</v>
+      </c>
       <c r="B13" s="54"/>
       <c r="C13" s="49"/>
-      <c r="D13" s="59" t="s">
+      <c r="D13" s="60" t="s">
         <v>19</v>
       </c>
       <c r="E13" s="49"/>
       <c r="F13" s="50"/>
       <c r="H13" s="9"/>
-      <c r="I13" s="61" t="s">
+      <c r="I13" s="62" t="s">
         <v>19</v>
       </c>
       <c r="J13" s="19"/>
@@ -2928,18 +2882,18 @@
       <c r="O13" s="1"/>
       <c r="P13" s="19"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1"/>
       <c r="B14" s="54"/>
       <c r="C14" s="49"/>
-      <c r="D14" s="59" t="s">
+      <c r="D14" s="60" t="s">
         <v>19</v>
       </c>
       <c r="E14" s="49"/>
       <c r="F14" s="50"/>
       <c r="H14" s="9"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="62" t="s">
+      <c r="J14" s="63" t="s">
         <v>19</v>
       </c>
       <c r="L14" s="9"/>
@@ -2950,9 +2904,9 @@
       <c r="O14" s="1"/>
       <c r="P14" s="19"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="63" t="s">
-        <v>57</v>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="59" t="s">
+        <v>60</v>
       </c>
       <c r="B15" s="54"/>
       <c r="C15" s="49"/>
@@ -2974,7 +2928,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="19"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="44" t="s">
         <v>27</v>
       </c>
@@ -2998,7 +2952,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="44" t="s">
         <v>27</v>
       </c>
@@ -3022,7 +2976,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="44" t="s">
         <v>27</v>
       </c>
@@ -3046,7 +3000,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="67"/>
       <c r="C19" s="68"/>
       <c r="D19" s="68"/>
@@ -3082,10 +3036,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:P13"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K37" activeCellId="0" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3106,12 +3060,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="21.71"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -3128,15 +3084,15 @@
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>11</v>
@@ -3145,7 +3101,7 @@
         <v>10</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>15</v>
@@ -3166,7 +3122,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="47"/>
       <c r="D5" s="20"/>
       <c r="F5" s="47"/>
@@ -3180,7 +3136,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="44" t="s">
         <v>27</v>
       </c>
@@ -3205,14 +3161,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="9"/>
-      <c r="C7" s="61" t="s">
+      <c r="C7" s="62" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="60" t="s">
+      <c r="F7" s="61" t="s">
         <v>19</v>
       </c>
       <c r="G7" s="1"/>
@@ -3228,15 +3184,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="9"/>
-      <c r="C8" s="61" t="s">
+      <c r="C8" s="62" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="1"/>
       <c r="F8" s="9"/>
-      <c r="G8" s="61" t="s">
+      <c r="G8" s="62" t="s">
         <v>19</v>
       </c>
       <c r="H8" s="19"/>
@@ -3248,16 +3204,16 @@
       <c r="M8" s="1"/>
       <c r="N8" s="19"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="9"/>
-      <c r="C9" s="61" t="s">
+      <c r="C9" s="62" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="1"/>
       <c r="F9" s="9"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="62" t="s">
+      <c r="H9" s="63" t="s">
         <v>19</v>
       </c>
       <c r="J9" s="9"/>
@@ -3268,14 +3224,14 @@
       <c r="M9" s="1"/>
       <c r="N9" s="19"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="9"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="62" t="s">
+      <c r="D10" s="63" t="s">
         <v>19</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="60" t="s">
+      <c r="F10" s="61" t="s">
         <v>19</v>
       </c>
       <c r="G10" s="1"/>
@@ -3288,15 +3244,15 @@
       <c r="M10" s="1"/>
       <c r="N10" s="19"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="9"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="62" t="s">
+      <c r="D11" s="63" t="s">
         <v>19</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="9"/>
-      <c r="G11" s="61" t="s">
+      <c r="G11" s="62" t="s">
         <v>19</v>
       </c>
       <c r="H11" s="19"/>
@@ -3308,16 +3264,16 @@
       <c r="M11" s="1"/>
       <c r="N11" s="19"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="9"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="62" t="s">
+      <c r="D12" s="63" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="9"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="62" t="s">
+      <c r="H12" s="63" t="s">
         <v>19</v>
       </c>
       <c r="J12" s="9"/>
@@ -3328,7 +3284,7 @@
       <c r="M12" s="1"/>
       <c r="N12" s="19"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="67"/>
       <c r="C13" s="68"/>
       <c r="D13" s="27"/>
@@ -3364,8 +3320,8 @@
   </sheetPr>
   <dimension ref="B2:G38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3380,193 +3336,193 @@
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="37" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="41" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="32.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="37" t="s">
+      <c r="D4" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="41" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="32.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="41" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="32.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="41" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="37" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F7" s="41" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="37" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F8" s="41" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="32.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="41" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="32.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="37" t="s">
-        <v>83</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="41" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="37" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>7</v>
@@ -3574,13 +3530,13 @@
     </row>
     <row r="12" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="37" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>7</v>
@@ -3588,13 +3544,13 @@
     </row>
     <row r="13" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="37" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>7</v>
@@ -3602,13 +3558,13 @@
     </row>
     <row r="14" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="37" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>7</v>
@@ -3616,10 +3572,10 @@
     </row>
     <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="37" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>4</v>
@@ -3630,10 +3586,10 @@
     </row>
     <row r="16" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="37" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>4</v>
@@ -3641,13 +3597,16 @@
       <c r="E16" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="32.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F16" s="69" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="37" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>4</v>
@@ -3656,18 +3615,15 @@
         <v>7</v>
       </c>
       <c r="F17" s="69" t="s">
-        <v>89</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="37" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>4</v>
@@ -3678,10 +3634,10 @@
     </row>
     <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="37" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>4</v>
@@ -3692,10 +3648,10 @@
     </row>
     <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="37" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>4</v>
@@ -3704,18 +3660,15 @@
         <v>7</v>
       </c>
       <c r="F20" s="69" t="s">
-        <v>90</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="37" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>4</v>
@@ -3726,10 +3679,10 @@
     </row>
     <row r="22" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="37" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>4</v>
@@ -3740,10 +3693,10 @@
     </row>
     <row r="23" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="37" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>4</v>
@@ -3754,10 +3707,10 @@
     </row>
     <row r="24" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="37" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>4</v>
@@ -3768,10 +3721,10 @@
     </row>
     <row r="25" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="37" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>4</v>
@@ -3782,10 +3735,10 @@
     </row>
     <row r="26" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="37" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>4</v>
@@ -3796,10 +3749,10 @@
     </row>
     <row r="27" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="37" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>5</v>
@@ -3810,10 +3763,10 @@
     </row>
     <row r="28" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="37" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>5</v>
@@ -3824,10 +3777,10 @@
     </row>
     <row r="29" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="37" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>5</v>
@@ -3838,10 +3791,10 @@
     </row>
     <row r="30" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="37" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>5</v>
@@ -3852,10 +3805,10 @@
     </row>
     <row r="31" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="37" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>5</v>
@@ -3866,10 +3819,10 @@
     </row>
     <row r="32" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="37" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>5</v>
@@ -3880,10 +3833,10 @@
     </row>
     <row r="33" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="37" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>5</v>
@@ -3894,10 +3847,10 @@
     </row>
     <row r="34" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="37" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>5</v>
@@ -3908,10 +3861,10 @@
     </row>
     <row r="35" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="37" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>5</v>
@@ -3922,10 +3875,10 @@
     </row>
     <row r="36" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="37" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>5</v>
@@ -3936,10 +3889,10 @@
     </row>
     <row r="37" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="37" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>5</v>
@@ -3950,10 +3903,10 @@
     </row>
     <row r="38" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="37" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>5</v>
@@ -3972,8 +3925,6 @@
     <hyperlink ref="G8" r:id="rId6" display="student19example@gmail.com"/>
     <hyperlink ref="G9" r:id="rId7" display="student19example@gmail.com"/>
     <hyperlink ref="G10" r:id="rId8" display="student19example@gmail.com"/>
-    <hyperlink ref="G17" r:id="rId9" display="student19example@gmail.com"/>
-    <hyperlink ref="G20" r:id="rId10" display="student19example@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -3983,175 +3934,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008A3605F12E6A764BA5E1F34B3DF10AD4" ma:contentTypeVersion="4" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="3323ec1b47b0987ad304cb442d78f841">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="81911cca-d972-4dec-b3a2-9564dbd2b986" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e2f652025f962b662e7ab9b23cee5ba3" ns2:_="">
-    <xsd:import namespace="81911cca-d972-4dec-b3a2-9564dbd2b986"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="81911cca-d972-4dec-b3a2-9564dbd2b986" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Inhoudstype"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titel"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E54E87A7-9B30-4E0D-9CFA-3592918BEA6A}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDF42566-0CDC-4DE2-9839-F4F14CBFA893}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA01DAD9-0254-47AE-A8BB-4204AFD839EE}"/>
 </file>
</xml_diff>

<commit_message>
Update badge distribution and overview
</commit_message>
<xml_diff>
--- a/test case overzicht surf.xlsx
+++ b/test case overzicht surf.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="BadgeClass CRUD" sheetId="1" state="visible" r:id="rId3"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="110">
   <si>
     <t xml:space="preserve">Onderwijsinstelling</t>
   </si>
@@ -177,9 +177,6 @@
     <t xml:space="preserve">Badge valideren - invalide</t>
   </si>
   <si>
-    <t xml:space="preserve">low prio</t>
-  </si>
-  <si>
     <t xml:space="preserve">Badge intrekken - MBO</t>
   </si>
   <si>
@@ -216,6 +213,9 @@
     <t xml:space="preserve">Instelling</t>
   </si>
   <si>
+    <t xml:space="preserve">Issuer</t>
+  </si>
+  <si>
     <t xml:space="preserve">Badges</t>
   </si>
   <si>
@@ -231,6 +231,18 @@
     <t xml:space="preserve">Verwijderen</t>
   </si>
   <si>
+    <t xml:space="preserve">UserManagement → Issuers → Read</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserManagement → Issuers → Create</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserManagement → Issuers → Update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserManagement → Issuers → Delete</t>
+  </si>
+  <si>
     <t xml:space="preserve">Teacher → BadgeInteraction → BadgeCreation</t>
   </si>
   <si>
@@ -249,7 +261,7 @@
     <t xml:space="preserve">Issuer group</t>
   </si>
   <si>
-    <t xml:space="preserve">Issuer</t>
+    <t xml:space="preserve">staff user</t>
   </si>
   <si>
     <t xml:space="preserve">InstitutionAdmin → EntityControl → Issuergroup → Create</t>
@@ -258,7 +270,7 @@
     <t xml:space="preserve">InstitutionAdmin → EntityControl → Issuergroup → Edit</t>
   </si>
   <si>
-    <t xml:space="preserve">EntityControl → UserManagement → Invite new user</t>
+    <t xml:space="preserve">EntityControl → UserManagement →  WOUser</t>
   </si>
   <si>
     <t xml:space="preserve">NOTE: all tests were performed on university-example, which is a WO institution</t>
@@ -267,12 +279,6 @@
     <t xml:space="preserve">Badgename</t>
   </si>
   <si>
-    <t xml:space="preserve">Instituition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Level</t>
-  </si>
-  <si>
     <t xml:space="preserve">Badgetype</t>
   </si>
   <si>
@@ -282,15 +288,12 @@
     <t xml:space="preserve">Account</t>
   </si>
   <si>
+    <t xml:space="preserve">NOTES:</t>
+  </si>
+  <si>
     <t xml:space="preserve">Law and Politics</t>
   </si>
   <si>
-    <t xml:space="preserve">university-example.org</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WO</t>
-  </si>
-  <si>
     <t xml:space="preserve">Receive by Student → Backpack → ReceiveBadge</t>
   </si>
   <si>
@@ -309,6 +312,9 @@
     <t xml:space="preserve">Reward by Student → Backpack → ReceiveBadge</t>
   </si>
   <si>
+    <t xml:space="preserve">Used to login by Student → Logout</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cognitive Psychology</t>
   </si>
   <si>
@@ -324,6 +330,9 @@
     <t xml:space="preserve">Request by Student → BasicsCatalog</t>
   </si>
   <si>
+    <t xml:space="preserve">Used by anonymous to look at</t>
+  </si>
+  <si>
     <t xml:space="preserve">Introduction to Political Science</t>
   </si>
   <si>
@@ -339,34 +348,21 @@
     <t xml:space="preserve">Growth and Development</t>
   </si>
   <si>
+    <t xml:space="preserve">Read by Teacher → BadgeInteraction → SeeBadge</t>
+  </si>
+  <si>
     <t xml:space="preserve">Regulation and Integration</t>
   </si>
   <si>
     <t xml:space="preserve">Digestion and Defense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Harvard-example.edu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Read by Teacher → BadgeInteraction → SeeBadge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Read by Student → BasicsCatalog</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Read by Anonymous → Catalog</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yale-uni-example.edu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -597,17 +593,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -678,7 +674,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -694,11 +690,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -738,6 +734,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -755,10 +755,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -774,10 +770,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -842,6 +834,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -912,6 +908,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="11" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1103,28 +1103,28 @@
   </sheetPr>
   <dimension ref="A3:S35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E49" activeCellId="0" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="1" width="17.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="11.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="1" width="19.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="10.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="3.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="2" width="17.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="2" width="11.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="2" width="19.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="10.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="10.57"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="1" t="n">
         <f aca="false">COUNTA(B5:B35)</f>
         <v>31</v>
       </c>
@@ -1177,7 +1177,7 @@
       <c r="K4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="M4" s="5" t="s">
@@ -1228,24 +1228,33 @@
       <c r="R5" s="15"/>
       <c r="S5" s="16"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1"/>
       <c r="B6" s="20" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>19</v>
       </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
       <c r="F6" s="9" t="s">
         <v>19</v>
       </c>
+      <c r="G6" s="2"/>
       <c r="H6" s="21"/>
+      <c r="I6" s="2"/>
       <c r="J6" s="9"/>
-      <c r="K6" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="K6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
       <c r="N6" s="22"/>
+      <c r="O6" s="0"/>
       <c r="P6" s="9"/>
-      <c r="R6" s="1" t="s">
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="S6" s="21"/>
@@ -1262,17 +1271,18 @@
       </c>
       <c r="H7" s="21"/>
       <c r="J7" s="9"/>
-      <c r="L7" s="1" t="s">
+      <c r="L7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N7" s="22"/>
       <c r="P7" s="9"/>
-      <c r="Q7" s="1" t="s">
+      <c r="Q7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="S7" s="21"/>
     </row>
-    <row r="8" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="12"/>
       <c r="B8" s="13" t="s">
         <v>19</v>
       </c>
@@ -1294,6 +1304,7 @@
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
       <c r="N8" s="23"/>
+      <c r="O8" s="12"/>
       <c r="P8" s="14" t="s">
         <v>19</v>
       </c>
@@ -1301,25 +1312,33 @@
       <c r="R8" s="15"/>
       <c r="S8" s="16"/>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1"/>
       <c r="B9" s="20" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>19</v>
       </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
       <c r="F9" s="9"/>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="21"/>
+      <c r="I9" s="2"/>
       <c r="J9" s="9"/>
-      <c r="K9" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="K9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
       <c r="N9" s="22"/>
+      <c r="O9" s="0"/>
       <c r="P9" s="9"/>
-      <c r="R9" s="1" t="s">
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2" t="s">
         <v>19</v>
       </c>
       <c r="S9" s="21"/>
@@ -1332,22 +1351,23 @@
         <v>19</v>
       </c>
       <c r="F10" s="9"/>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H10" s="21"/>
       <c r="J10" s="9"/>
-      <c r="L10" s="1" t="s">
+      <c r="L10" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N10" s="22"/>
       <c r="P10" s="9"/>
-      <c r="Q10" s="1" t="s">
+      <c r="Q10" s="2" t="s">
         <v>19</v>
       </c>
       <c r="S10" s="21"/>
     </row>
-    <row r="11" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="12"/>
       <c r="B11" s="13" t="s">
         <v>19</v>
       </c>
@@ -1369,6 +1389,7 @@
       <c r="L11" s="15"/>
       <c r="M11" s="15"/>
       <c r="N11" s="23"/>
+      <c r="O11" s="12"/>
       <c r="P11" s="14" t="s">
         <v>19</v>
       </c>
@@ -1376,24 +1397,33 @@
       <c r="R11" s="15"/>
       <c r="S11" s="16"/>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
       <c r="B12" s="20" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>19</v>
       </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
       <c r="F12" s="9"/>
+      <c r="G12" s="2"/>
       <c r="H12" s="21" t="s">
         <v>19</v>
       </c>
+      <c r="I12" s="2"/>
       <c r="J12" s="9"/>
-      <c r="K12" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="K12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
       <c r="N12" s="22"/>
+      <c r="O12" s="0"/>
       <c r="P12" s="9"/>
-      <c r="R12" s="1" t="s">
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="S12" s="21"/>
@@ -1410,17 +1440,18 @@
         <v>19</v>
       </c>
       <c r="J13" s="9"/>
-      <c r="L13" s="1" t="s">
+      <c r="L13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N13" s="22"/>
       <c r="P13" s="9"/>
-      <c r="Q13" s="1" t="s">
+      <c r="Q13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="S13" s="21"/>
     </row>
-    <row r="14" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="12"/>
       <c r="B14" s="13" t="s">
         <v>19</v>
       </c>
@@ -1442,6 +1473,7 @@
       <c r="L14" s="15"/>
       <c r="M14" s="15"/>
       <c r="N14" s="23"/>
+      <c r="O14" s="12"/>
       <c r="P14" s="14" t="s">
         <v>19</v>
       </c>
@@ -1454,7 +1486,7 @@
         <v>19</v>
       </c>
       <c r="C15" s="9"/>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F15" s="9" t="s">
@@ -1462,12 +1494,12 @@
       </c>
       <c r="H15" s="21"/>
       <c r="J15" s="9"/>
-      <c r="K15" s="1" t="s">
+      <c r="K15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N15" s="22"/>
       <c r="P15" s="9"/>
-      <c r="R15" s="1" t="s">
+      <c r="R15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="S15" s="21"/>
@@ -1477,7 +1509,7 @@
         <v>19</v>
       </c>
       <c r="C16" s="9"/>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F16" s="9" t="s">
@@ -1485,17 +1517,18 @@
       </c>
       <c r="H16" s="21"/>
       <c r="J16" s="9"/>
-      <c r="L16" s="1" t="s">
+      <c r="L16" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N16" s="22"/>
       <c r="P16" s="9"/>
-      <c r="Q16" s="1" t="s">
+      <c r="Q16" s="2" t="s">
         <v>19</v>
       </c>
       <c r="S16" s="21"/>
     </row>
-    <row r="17" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="12"/>
       <c r="B17" s="13" t="s">
         <v>19</v>
       </c>
@@ -1517,6 +1550,7 @@
       <c r="L17" s="15"/>
       <c r="M17" s="15"/>
       <c r="N17" s="23"/>
+      <c r="O17" s="12"/>
       <c r="P17" s="14" t="s">
         <v>19</v>
       </c>
@@ -1529,21 +1563,21 @@
         <v>19</v>
       </c>
       <c r="C18" s="9"/>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F18" s="9"/>
-      <c r="G18" s="1" t="s">
+      <c r="G18" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H18" s="21"/>
       <c r="J18" s="9"/>
-      <c r="K18" s="1" t="s">
+      <c r="K18" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N18" s="22"/>
       <c r="P18" s="9"/>
-      <c r="R18" s="1" t="s">
+      <c r="R18" s="2" t="s">
         <v>19</v>
       </c>
       <c r="S18" s="21"/>
@@ -1553,21 +1587,21 @@
         <v>19</v>
       </c>
       <c r="C19" s="9"/>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F19" s="9"/>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H19" s="21"/>
       <c r="J19" s="9"/>
-      <c r="L19" s="1" t="s">
+      <c r="L19" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N19" s="22"/>
       <c r="P19" s="9"/>
-      <c r="Q19" s="1" t="s">
+      <c r="Q19" s="2" t="s">
         <v>19</v>
       </c>
       <c r="S19" s="21"/>
@@ -1608,7 +1642,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="9"/>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="9"/>
@@ -1616,12 +1650,12 @@
         <v>19</v>
       </c>
       <c r="J21" s="9"/>
-      <c r="K21" s="1" t="s">
+      <c r="K21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N21" s="22"/>
       <c r="P21" s="9"/>
-      <c r="R21" s="1" t="s">
+      <c r="R21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="S21" s="21"/>
@@ -1631,7 +1665,7 @@
         <v>19</v>
       </c>
       <c r="C22" s="9"/>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F22" s="9"/>
@@ -1639,17 +1673,18 @@
         <v>19</v>
       </c>
       <c r="J22" s="9"/>
-      <c r="L22" s="1" t="s">
+      <c r="L22" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N22" s="22"/>
       <c r="P22" s="9"/>
-      <c r="Q22" s="1" t="s">
+      <c r="Q22" s="2" t="s">
         <v>19</v>
       </c>
       <c r="S22" s="21"/>
     </row>
-    <row r="23" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="12"/>
       <c r="B23" s="13" t="s">
         <v>19</v>
       </c>
@@ -1671,6 +1706,7 @@
       <c r="L23" s="15"/>
       <c r="M23" s="15"/>
       <c r="N23" s="23"/>
+      <c r="O23" s="12"/>
       <c r="P23" s="14" t="s">
         <v>19</v>
       </c>
@@ -1699,7 +1735,7 @@
       </c>
       <c r="N24" s="22"/>
       <c r="P24" s="9"/>
-      <c r="R24" s="1" t="s">
+      <c r="R24" s="2" t="s">
         <v>19</v>
       </c>
       <c r="S24" s="21"/>
@@ -1721,12 +1757,12 @@
       <c r="H25" s="21"/>
       <c r="J25" s="9"/>
       <c r="K25" s="26"/>
-      <c r="L25" s="1" t="s">
+      <c r="L25" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N25" s="22"/>
       <c r="P25" s="9"/>
-      <c r="R25" s="1" t="s">
+      <c r="R25" s="2" t="s">
         <v>19</v>
       </c>
       <c r="S25" s="21"/>
@@ -1739,7 +1775,7 @@
         <v>19</v>
       </c>
       <c r="C26" s="9"/>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F26" s="9" t="s">
@@ -1751,12 +1787,13 @@
         <v>19</v>
       </c>
       <c r="P26" s="9"/>
-      <c r="Q26" s="1" t="s">
+      <c r="Q26" s="2" t="s">
         <v>19</v>
       </c>
       <c r="S26" s="21"/>
     </row>
-    <row r="27" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="12"/>
       <c r="B27" s="13" t="s">
         <v>19</v>
       </c>
@@ -1778,6 +1815,7 @@
       <c r="L27" s="15"/>
       <c r="M27" s="15"/>
       <c r="N27" s="23"/>
+      <c r="O27" s="12"/>
       <c r="P27" s="14" t="s">
         <v>19</v>
       </c>
@@ -1797,7 +1835,7 @@
         <v>19</v>
       </c>
       <c r="F28" s="9"/>
-      <c r="G28" s="1" t="s">
+      <c r="G28" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H28" s="21"/>
@@ -1807,7 +1845,7 @@
       </c>
       <c r="N28" s="22"/>
       <c r="P28" s="9"/>
-      <c r="R28" s="1" t="s">
+      <c r="R28" s="2" t="s">
         <v>19</v>
       </c>
       <c r="S28" s="21"/>
@@ -1820,11 +1858,11 @@
         <v>19</v>
       </c>
       <c r="C29" s="9"/>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F29" s="9"/>
-      <c r="G29" s="1" t="s">
+      <c r="G29" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H29" s="21"/>
@@ -1833,7 +1871,7 @@
         <v>19</v>
       </c>
       <c r="P29" s="9"/>
-      <c r="R29" s="1" t="s">
+      <c r="R29" s="2" t="s">
         <v>19</v>
       </c>
       <c r="S29" s="21"/>
@@ -1846,27 +1884,28 @@
         <v>19</v>
       </c>
       <c r="C30" s="9"/>
-      <c r="E30" s="1" t="s">
+      <c r="E30" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F30" s="9"/>
-      <c r="G30" s="1" t="s">
+      <c r="G30" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H30" s="21"/>
       <c r="J30" s="9"/>
       <c r="K30" s="26"/>
-      <c r="L30" s="1" t="s">
+      <c r="L30" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N30" s="22"/>
       <c r="P30" s="9"/>
-      <c r="Q30" s="1" t="s">
+      <c r="Q30" s="2" t="s">
         <v>19</v>
       </c>
       <c r="S30" s="21"/>
     </row>
-    <row r="31" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="12"/>
       <c r="B31" s="13" t="s">
         <v>19</v>
       </c>
@@ -1888,6 +1927,7 @@
       <c r="L31" s="15"/>
       <c r="M31" s="15"/>
       <c r="N31" s="23"/>
+      <c r="O31" s="12"/>
       <c r="P31" s="14" t="s">
         <v>19</v>
       </c>
@@ -1903,7 +1943,7 @@
         <v>19</v>
       </c>
       <c r="C32" s="9"/>
-      <c r="E32" s="1" t="s">
+      <c r="E32" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F32" s="9"/>
@@ -1911,12 +1951,12 @@
         <v>19</v>
       </c>
       <c r="J32" s="9"/>
-      <c r="K32" s="1" t="s">
+      <c r="K32" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N32" s="22"/>
       <c r="P32" s="9"/>
-      <c r="R32" s="1" t="s">
+      <c r="R32" s="2" t="s">
         <v>19</v>
       </c>
       <c r="S32" s="21"/>
@@ -1929,7 +1969,7 @@
         <v>19</v>
       </c>
       <c r="C33" s="9"/>
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F33" s="9"/>
@@ -1941,7 +1981,7 @@
         <v>19</v>
       </c>
       <c r="P33" s="9"/>
-      <c r="R33" s="1" t="s">
+      <c r="R33" s="2" t="s">
         <v>19</v>
       </c>
       <c r="S33" s="21"/>
@@ -1954,7 +1994,7 @@
         <v>19</v>
       </c>
       <c r="C34" s="9"/>
-      <c r="E34" s="1" t="s">
+      <c r="E34" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F34" s="9"/>
@@ -1962,12 +2002,12 @@
         <v>19</v>
       </c>
       <c r="J34" s="9"/>
-      <c r="L34" s="1" t="s">
+      <c r="L34" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N34" s="22"/>
       <c r="P34" s="9"/>
-      <c r="Q34" s="1" t="s">
+      <c r="Q34" s="2" t="s">
         <v>19</v>
       </c>
       <c r="S34" s="21"/>
@@ -2014,417 +2054,433 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L11" activeCellId="0" sqref="L11"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="36.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="10.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="11.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="10.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="2" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="11.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="2" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="17.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="36.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="10.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="11.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
-      <c r="K3" s="5" t="s">
+      <c r="J3" s="4"/>
+      <c r="L3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="5"/>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
-        <f aca="false">COUNTA(A5:A21)</f>
+      <c r="B4" s="1" t="n">
+        <f aca="false">COUNTA(B5:B21)</f>
         <v>12</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="E4" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="32" t="s">
+      <c r="J4" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="L4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="M4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="N4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="O4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="O4" s="10" t="s">
+      <c r="P4" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="3"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="33"/>
-      <c r="I5" s="21"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="31"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="33"/>
+      <c r="J5" s="21"/>
+      <c r="L5" s="3"/>
       <c r="M5" s="31"/>
       <c r="N5" s="31"/>
-      <c r="O5" s="11"/>
-    </row>
-    <row r="6" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="15"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="11"/>
+    </row>
+    <row r="6" s="34" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="15"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="15" t="s">
+        <v>19</v>
+      </c>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
-      <c r="I6" s="16"/>
-      <c r="K6" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="14" t="s">
+        <v>19</v>
+      </c>
       <c r="M6" s="15"/>
       <c r="N6" s="15"/>
-      <c r="O6" s="23"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="21"/>
-      <c r="F7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="21"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="22"/>
-    </row>
-    <row r="8" s="34" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="23"/>
+    </row>
+    <row r="7" s="35" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0"/>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="0"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="22"/>
+    </row>
+    <row r="8" s="35" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="34"/>
+      <c r="B8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="16"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
-      <c r="H8" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="16"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="16"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="14" t="s">
+        <v>19</v>
+      </c>
       <c r="M8" s="15"/>
       <c r="N8" s="15"/>
-      <c r="O8" s="23"/>
-    </row>
-    <row r="9" s="39" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="36"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="23"/>
+    </row>
+    <row r="9" s="34" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="35"/>
+      <c r="B9" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>19</v>
+      </c>
       <c r="D9" s="37"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="J9" s="34"/>
-      <c r="K9" s="35"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="38" t="s">
+        <v>19</v>
+      </c>
       <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="38" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" s="39" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="26"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="39" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="35"/>
+      <c r="B10" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="21"/>
+      <c r="F10" s="26" t="s">
+        <v>19</v>
+      </c>
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
-      <c r="I10" s="21"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="26" t="s">
+        <v>19</v>
+      </c>
       <c r="N10" s="26"/>
-      <c r="O10" s="22"/>
-    </row>
-    <row r="11" s="34" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="26"/>
+      <c r="O10" s="26"/>
+      <c r="P10" s="22"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="34"/>
+      <c r="B11" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="21"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26" t="s">
+        <v>19</v>
+      </c>
       <c r="H11" s="26"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="M11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="26" t="s">
+        <v>19</v>
+      </c>
       <c r="N11" s="26"/>
-      <c r="O11" s="22"/>
-    </row>
-    <row r="12" s="39" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="26"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="22"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="35"/>
+      <c r="B12" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="21"/>
       <c r="F12" s="26"/>
       <c r="G12" s="26"/>
-      <c r="H12" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="I12" s="21"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="M12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="21"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="26" t="s">
+        <v>19</v>
+      </c>
       <c r="N12" s="26"/>
-      <c r="O12" s="22"/>
-    </row>
-    <row r="13" s="39" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="37"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="J13" s="34"/>
-      <c r="K13" s="35"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="22"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="35"/>
+      <c r="B13" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="36"/>
+      <c r="D13" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="38"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="34"/>
       <c r="L13" s="36"/>
-      <c r="M13" s="36"/>
-      <c r="N13" s="36"/>
-      <c r="O13" s="38" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" s="34" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="26"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="39" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="34"/>
+      <c r="B14" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>19</v>
+      </c>
       <c r="G14" s="26"/>
       <c r="H14" s="26"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="M14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="26" t="s">
+        <v>19</v>
+      </c>
       <c r="N14" s="26"/>
-      <c r="O14" s="22"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="22"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="26"/>
+      <c r="B15" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26" t="s">
+        <v>19</v>
+      </c>
       <c r="H15" s="26"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="M15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="26" t="s">
+        <v>19</v>
+      </c>
       <c r="N15" s="26"/>
-      <c r="O15" s="22"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="22"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="26"/>
+      <c r="B16" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="21" t="s">
+        <v>19</v>
+      </c>
       <c r="F16" s="26"/>
       <c r="G16" s="26"/>
-      <c r="H16" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="I16" s="21"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="M16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="21"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="26" t="s">
+        <v>19</v>
+      </c>
       <c r="N16" s="26"/>
-      <c r="O16" s="22"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="22"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="35"/>
+      <c r="B17" s="34" t="s">
+        <v>19</v>
+      </c>
       <c r="C17" s="36"/>
-      <c r="D17" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="J17" s="34"/>
-      <c r="K17" s="35"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" s="34"/>
       <c r="L17" s="36"/>
-      <c r="M17" s="36"/>
-      <c r="N17" s="36"/>
-      <c r="O17" s="38" t="s">
+      <c r="M17" s="37"/>
+      <c r="N17" s="37"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="39" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="27"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="28"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="29"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
       <c r="H18" s="28"/>
-      <c r="I18" s="29"/>
-      <c r="K18" s="27"/>
-      <c r="L18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="29"/>
+      <c r="L18" s="27"/>
       <c r="M18" s="28"/>
       <c r="N18" s="28"/>
-      <c r="O18" s="30"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:I3"/>
-    <mergeCell ref="K3:O3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="L3:P3"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2444,19 +2500,19 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="21.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="36.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="10.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="11.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="23.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="23.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2473,10 +2529,10 @@
       <c r="H2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D3" s="9" t="s">
@@ -2515,29 +2571,29 @@
       <c r="D5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
       <c r="H5" s="21"/>
       <c r="J5" s="43" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="24" t="s">
         <v>40</v>
       </c>
       <c r="B6" s="41" t="s">
         <v>41</v>
       </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="1"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="2"/>
       <c r="H6" s="21"/>
-      <c r="J6" s="45" t="s">
+      <c r="J6" s="44" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2551,42 +2607,42 @@
       <c r="D7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
       <c r="H7" s="21"/>
-      <c r="J7" s="46" t="s">
+      <c r="J7" s="45" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="24" t="s">
         <v>45</v>
       </c>
       <c r="B8" s="41" t="s">
         <v>46</v>
       </c>
       <c r="D8" s="9"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1" t="s">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H8" s="21"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B9" s="43" t="s">
         <v>48</v>
       </c>
       <c r="D9" s="9"/>
-      <c r="E9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="E9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
       <c r="H9" s="21"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2594,56 +2650,50 @@
         <v>49</v>
       </c>
       <c r="D10" s="9"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="1"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="2"/>
       <c r="H10" s="21"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="D11" s="9"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="21"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="21"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" s="43" t="s">
+      <c r="D12" s="9"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="21"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="21"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="44" t="s">
+      <c r="B13" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="43" t="s">
-        <v>54</v>
-      </c>
       <c r="D13" s="9"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="1"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="2"/>
       <c r="H13" s="21"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2651,43 +2701,43 @@
         <v>37</v>
       </c>
       <c r="B14" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="21"/>
+    </row>
+    <row r="15" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="21"/>
-    </row>
-    <row r="15" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="47" t="s">
+      <c r="B15" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="48" t="s">
+      <c r="D15" s="9"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="21"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="21"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="50" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="46" t="s">
-        <v>58</v>
-      </c>
       <c r="D16" s="9"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="51" t="s">
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="50" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2702,8 +2752,8 @@
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D21" s="2" t="s">
-        <v>59</v>
+      <c r="D21" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2728,45 +2778,45 @@
   <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="37.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="4.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="2" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="10.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="11.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="22.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="40.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="4.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="10.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="11.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="22.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="35" t="s">
         <v>34</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
-      <c r="H3" s="52" t="s">
-        <v>61</v>
-      </c>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
+      <c r="H3" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
       <c r="M3" s="5" t="s">
         <v>3</v>
       </c>
@@ -2777,10 +2827,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>1</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>63</v>
@@ -2823,9 +2873,9 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="53"/>
+      <c r="B5" s="52"/>
       <c r="F5" s="22"/>
-      <c r="H5" s="53"/>
+      <c r="H5" s="52"/>
       <c r="K5" s="22"/>
       <c r="M5" s="3"/>
       <c r="N5" s="31"/>
@@ -2837,424 +2887,432 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="54" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="55"/>
-      <c r="H6" s="56" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="B6" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="54"/>
+      <c r="H6" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
       <c r="K6" s="21"/>
       <c r="M6" s="9"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="S6" s="45" t="s">
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="S6" s="44" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="54" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="55"/>
+      <c r="B7" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="54"/>
       <c r="H7" s="9"/>
-      <c r="I7" s="57" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="1"/>
+      <c r="I7" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="2"/>
       <c r="K7" s="21"/>
       <c r="M7" s="9"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="S7" s="46" t="s">
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="S7" s="45" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="50" t="s">
+      <c r="A8" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="54" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="55"/>
+      <c r="B8" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="54"/>
       <c r="H8" s="9"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="57" t="s">
+      <c r="I8" s="2"/>
+      <c r="J8" s="56" t="s">
         <v>19</v>
       </c>
       <c r="K8" s="21"/>
       <c r="M8" s="9"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="S8" s="46"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="S8" s="45"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="50" t="s">
+      <c r="A9" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="54" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="55"/>
+      <c r="B9" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="54"/>
       <c r="H9" s="9"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="58" t="s">
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="57" t="s">
         <v>19</v>
       </c>
       <c r="M9" s="9"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="51" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
-      <c r="B10" s="59"/>
-      <c r="C10" s="60" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="55"/>
-      <c r="H10" s="60" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="50" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="58"/>
+      <c r="C10" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="54"/>
+      <c r="H10" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
       <c r="K10" s="21"/>
       <c r="M10" s="9"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P10" s="1"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P10" s="2"/>
       <c r="Q10" s="21"/>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1"/>
-      <c r="B11" s="59"/>
-      <c r="C11" s="60" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="55"/>
+    <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="58"/>
+      <c r="C11" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="54"/>
       <c r="H11" s="9"/>
-      <c r="I11" s="60" t="s">
-        <v>19</v>
-      </c>
-      <c r="J11" s="1"/>
+      <c r="I11" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="2"/>
       <c r="K11" s="21"/>
       <c r="M11" s="9"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P11" s="1"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P11" s="2"/>
       <c r="Q11" s="21"/>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1"/>
-      <c r="B12" s="59"/>
-      <c r="C12" s="60" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="55"/>
+    <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="60" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="58"/>
+      <c r="C12" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="54"/>
       <c r="H12" s="9"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="60" t="s">
+      <c r="I12" s="2"/>
+      <c r="J12" s="59" t="s">
         <v>19</v>
       </c>
       <c r="K12" s="21"/>
       <c r="M12" s="9"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P12" s="1"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P12" s="2"/>
       <c r="Q12" s="21"/>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1"/>
-      <c r="B13" s="59"/>
-      <c r="C13" s="60" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="55"/>
+    <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="58"/>
+      <c r="C13" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="54"/>
       <c r="H13" s="9"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="60" t="s">
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="59" t="s">
         <v>19</v>
       </c>
       <c r="M13" s="9"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P13" s="1"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P13" s="2"/>
       <c r="Q13" s="21"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="61" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" s="59"/>
-      <c r="C14" s="49"/>
+        <v>72</v>
+      </c>
+      <c r="B14" s="58"/>
+      <c r="C14" s="48"/>
       <c r="D14" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="49"/>
-      <c r="F14" s="55"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="54"/>
       <c r="H14" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
       <c r="K14" s="21"/>
       <c r="M14" s="9"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P14" s="1"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P14" s="2"/>
       <c r="Q14" s="21"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="61" t="s">
-        <v>68</v>
-      </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="49"/>
+        <v>72</v>
+      </c>
+      <c r="B15" s="58"/>
+      <c r="C15" s="48"/>
       <c r="D15" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="49"/>
-      <c r="F15" s="55"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="54"/>
       <c r="H15" s="9"/>
       <c r="I15" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="1"/>
+      <c r="J15" s="2"/>
       <c r="K15" s="21"/>
       <c r="M15" s="9"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P15" s="1"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P15" s="2"/>
       <c r="Q15" s="21"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="61" t="s">
-        <v>69</v>
-      </c>
-      <c r="B16" s="59"/>
-      <c r="C16" s="49"/>
+        <v>73</v>
+      </c>
+      <c r="B16" s="58"/>
+      <c r="C16" s="48"/>
       <c r="D16" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="49"/>
-      <c r="F16" s="55"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="54"/>
       <c r="H16" s="9"/>
-      <c r="I16" s="1"/>
+      <c r="I16" s="2"/>
       <c r="J16" s="62" t="s">
         <v>19</v>
       </c>
       <c r="K16" s="21"/>
       <c r="M16" s="9"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P16" s="1"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P16" s="2"/>
       <c r="Q16" s="21"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="61" t="s">
-        <v>70</v>
-      </c>
-      <c r="B17" s="59"/>
-      <c r="C17" s="49"/>
+        <v>74</v>
+      </c>
+      <c r="B17" s="58"/>
+      <c r="C17" s="48"/>
       <c r="D17" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="49"/>
-      <c r="F17" s="55"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="54"/>
       <c r="H17" s="9"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
       <c r="K17" s="62" t="s">
         <v>19</v>
       </c>
       <c r="M17" s="9"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P17" s="1"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P17" s="2"/>
       <c r="Q17" s="21"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="61" t="s">
-        <v>71</v>
-      </c>
-      <c r="B18" s="59"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
+        <v>75</v>
+      </c>
+      <c r="B18" s="58"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
       <c r="E18" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="55"/>
+      <c r="F18" s="54"/>
       <c r="H18" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
       <c r="K18" s="21"/>
       <c r="M18" s="9"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P18" s="1"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P18" s="2"/>
       <c r="Q18" s="21"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="59"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
       <c r="F19" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="H19" s="56" t="s">
-        <v>19</v>
-      </c>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
+      <c r="H19" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
       <c r="K19" s="21"/>
       <c r="M19" s="9"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="51" t="s">
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="50" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="59"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
       <c r="F20" s="65" t="s">
         <v>19</v>
       </c>
       <c r="H20" s="9"/>
-      <c r="I20" s="57" t="s">
-        <v>19</v>
-      </c>
-      <c r="J20" s="1"/>
+      <c r="I20" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" s="2"/>
       <c r="K20" s="21"/>
       <c r="M20" s="9"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="51" t="s">
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="50" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="50" t="s">
+      <c r="A21" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="59"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
+      <c r="B21" s="58"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
       <c r="F21" s="65" t="s">
         <v>19</v>
       </c>
       <c r="H21" s="9"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="57" t="s">
+      <c r="I21" s="2"/>
+      <c r="J21" s="56" t="s">
         <v>19</v>
       </c>
       <c r="K21" s="21"/>
       <c r="M21" s="9"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="51"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="50"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="50" t="s">
+      <c r="A22" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="59"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
       <c r="F22" s="65" t="s">
         <v>19</v>
       </c>
       <c r="H22" s="9"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="58" t="s">
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="57" t="s">
         <v>19</v>
       </c>
       <c r="M22" s="9"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="51" t="s">
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="50" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3295,89 +3353,93 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="28.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="8.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="6.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="10.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="11.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="21.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="10.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="11.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="21.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="F3" s="4" t="s">
+      <c r="E3" s="4"/>
+      <c r="G3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-      <c r="J3" s="5" t="s">
+      <c r="I3" s="4"/>
+      <c r="K3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="5"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F4" s="6" t="s">
+      <c r="E4" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="K4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="L4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="M4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="P4" s="41" t="s">
+      <c r="Q4" s="41" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3385,202 +3447,284 @@
       <c r="B5" s="68"/>
       <c r="C5" s="69"/>
       <c r="D5" s="70"/>
-      <c r="F5" s="53"/>
-      <c r="H5" s="22"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="72"/>
+      <c r="E5" s="70"/>
+      <c r="G5" s="52"/>
+      <c r="I5" s="22"/>
+      <c r="K5" s="71"/>
       <c r="L5" s="72"/>
       <c r="M5" s="72"/>
-      <c r="N5" s="73"/>
-      <c r="P5" s="43" t="s">
+      <c r="N5" s="72"/>
+      <c r="O5" s="73"/>
+      <c r="Q5" s="43" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="54" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="54" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="49"/>
-      <c r="H6" s="55"/>
-      <c r="J6" s="74"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="69"/>
-      <c r="M6" s="49"/>
-      <c r="N6" s="75" t="s">
-        <v>19</v>
-      </c>
-      <c r="P6" s="45" t="s">
+      <c r="B6" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="48"/>
+      <c r="I6" s="54"/>
+      <c r="K6" s="74"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="69"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="75" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q6" s="44" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="47" t="s">
-        <v>75</v>
+      <c r="A7" s="46" t="s">
+        <v>79</v>
       </c>
       <c r="B7" s="74"/>
       <c r="C7" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="55"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="77" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="49"/>
-      <c r="H7" s="55"/>
-      <c r="J7" s="74"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="M7" s="49"/>
-      <c r="N7" s="55"/>
-      <c r="P7" s="46" t="s">
+      <c r="D7" s="48"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="77" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="48"/>
+      <c r="I7" s="54"/>
+      <c r="K7" s="74"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" s="48"/>
+      <c r="O7" s="54"/>
+      <c r="Q7" s="45" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="47" t="s">
-        <v>76</v>
+      <c r="A8" s="46" t="s">
+        <v>80</v>
       </c>
       <c r="B8" s="74"/>
       <c r="C8" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="55"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="74"/>
-      <c r="G8" s="76" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="55"/>
-      <c r="J8" s="74"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8" s="49"/>
-      <c r="N8" s="55"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="74"/>
+      <c r="H8" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="54"/>
+      <c r="K8" s="74"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="48"/>
+      <c r="O8" s="54"/>
     </row>
     <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="47" t="s">
-        <v>56</v>
+      <c r="A9" s="46" t="s">
+        <v>55</v>
       </c>
       <c r="B9" s="74"/>
       <c r="C9" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="55"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="74"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="78" t="s">
-        <v>19</v>
-      </c>
-      <c r="J9" s="74"/>
-      <c r="K9" s="49"/>
-      <c r="L9" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="M9" s="49"/>
-      <c r="N9" s="55"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D9" s="48"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="78" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="74"/>
+      <c r="L9" s="48"/>
+      <c r="M9" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="N9" s="48"/>
+      <c r="O9" s="54"/>
+    </row>
+    <row r="10" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="46" t="s">
+        <v>70</v>
+      </c>
       <c r="B10" s="74"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="78" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="77" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="49"/>
-      <c r="H10" s="55"/>
-      <c r="J10" s="74"/>
-      <c r="K10" s="49"/>
-      <c r="L10" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10" s="49"/>
-      <c r="N10" s="55"/>
-    </row>
-    <row r="11" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="47" t="s">
-        <v>77</v>
+      <c r="C10" s="48"/>
+      <c r="D10" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="54"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="77" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="48"/>
+      <c r="I10" s="54"/>
+      <c r="K10" s="74"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="N10" s="48"/>
+      <c r="O10" s="54"/>
+    </row>
+    <row r="11" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="60" t="s">
+        <v>69</v>
       </c>
       <c r="B11" s="74"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="78" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="76" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="55"/>
-      <c r="J11" s="74"/>
-      <c r="K11" s="49"/>
-      <c r="L11" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="M11" s="49"/>
-      <c r="N11" s="55"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="48"/>
+      <c r="D11" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="54"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="54"/>
+      <c r="K11" s="74"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="N11" s="48"/>
+      <c r="O11" s="54"/>
+    </row>
+    <row r="12" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="46" t="s">
+        <v>71</v>
+      </c>
       <c r="B12" s="74"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="78" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="78" t="s">
-        <v>19</v>
-      </c>
-      <c r="J12" s="74"/>
-      <c r="K12" s="49"/>
-      <c r="L12" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="M12" s="49"/>
-      <c r="N12" s="55"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="54"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="74"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="78" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="74"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="N12" s="48"/>
+      <c r="O12" s="54"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="66"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="30"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="30"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="29"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
-        <v>78</v>
+      <c r="B13" s="74"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="78" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="77" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="48"/>
+      <c r="I13" s="54"/>
+      <c r="K13" s="74"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="O13" s="54"/>
+    </row>
+    <row r="14" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="74"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="78" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="74"/>
+      <c r="H14" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="54"/>
+      <c r="K14" s="74"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="O14" s="54"/>
+    </row>
+    <row r="15" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="74"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="78" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="74"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="78" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" s="74"/>
+      <c r="L15" s="48"/>
+      <c r="M15" s="48"/>
+      <c r="N15" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="O15" s="54"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="30"/>
+      <c r="G16" s="66"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="30"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="29"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B3:D3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="K3:O3"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3597,613 +3741,233 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:G38"/>
+  <dimension ref="B2:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M11" activeCellId="0" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="15.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="21.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="6.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="9.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="48.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="27.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="48.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="27.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="30.68"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>84</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="40" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="44" t="s">
-        <v>88</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="D3" s="24" t="s">
         <v>89</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="44" t="s">
-        <v>91</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="40" t="s">
-        <v>92</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="44" t="s">
-        <v>93</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>89</v>
+      <c r="D5" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="40" t="s">
-        <v>94</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E6" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="44" t="s">
-        <v>95</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>89</v>
+      <c r="D6" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="40" t="s">
-        <v>96</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E7" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="44" t="s">
-        <v>95</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>89</v>
+      <c r="D7" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="40" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E8" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="44" t="s">
-        <v>98</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>89</v>
+      <c r="D8" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="40" t="s">
-        <v>99</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="44" t="s">
-        <v>100</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>89</v>
+      <c r="D9" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="40" t="s">
-        <v>101</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="44" t="s">
-        <v>100</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>89</v>
+      <c r="D10" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="40" t="s">
-        <v>102</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E11" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="D11" s="79"/>
     </row>
     <row r="12" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E12" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="D12" s="80" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="40" t="s">
-        <v>105</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E14" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="40" t="s">
-        <v>85</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="40" t="s">
-        <v>90</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="79" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="40" t="s">
-        <v>92</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="79" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="40" t="s">
-        <v>94</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="40" t="s">
-        <v>96</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="40" t="s">
-        <v>97</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="79" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="40" t="s">
-        <v>99</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="40" t="s">
-        <v>101</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="40" t="s">
-        <v>102</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="40" t="s">
-        <v>105</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="40" t="s">
-        <v>85</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="40" t="s">
-        <v>90</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="40" t="s">
-        <v>92</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="40" t="s">
-        <v>94</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="40" t="s">
-        <v>96</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="40" t="s">
-        <v>97</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="40" t="s">
-        <v>99</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="40" t="s">
-        <v>101</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="40" t="s">
-        <v>102</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="40" t="s">
-        <v>105</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
+    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1" display="student19example@gmail.com"/>
-    <hyperlink ref="G4" r:id="rId2" display="student19example@gmail.com"/>
-    <hyperlink ref="G5" r:id="rId3" display="student19example@gmail.com"/>
-    <hyperlink ref="G6" r:id="rId4" display="student19example@gmail.com"/>
-    <hyperlink ref="G7" r:id="rId5" display="student19example@gmail.com"/>
-    <hyperlink ref="G8" r:id="rId6" display="student19example@gmail.com"/>
-    <hyperlink ref="G9" r:id="rId7" display="student19example@gmail.com"/>
-    <hyperlink ref="G10" r:id="rId8" display="student19example@gmail.com"/>
+    <hyperlink ref="E3" r:id="rId1" display="student19example@gmail.com"/>
+    <hyperlink ref="E4" r:id="rId2" display="student19example@gmail.com"/>
+    <hyperlink ref="E5" r:id="rId3" display="student19example@gmail.com"/>
+    <hyperlink ref="E6" r:id="rId4" display="student19example@gmail.com"/>
+    <hyperlink ref="E7" r:id="rId5" display="student19example@gmail.com"/>
+    <hyperlink ref="E8" r:id="rId6" display="student19example@gmail.com"/>
+    <hyperlink ref="E9" r:id="rId7" display="student19example@gmail.com"/>
+    <hyperlink ref="E10" r:id="rId8" display="student19example@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>